<commit_message>
Added tests for Kubernetes tab
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/LocatorDictionary/DownloadServerPageLocators.xlsx
+++ b/src/main/resources/CompilerDictionary/LocatorDictionary/DownloadServerPageLocators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/src/main/resources/CompilerDictionary/LocatorDictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4846F4-30C5-8948-9EB4-48F1994EF02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02EAAA7-1BDC-C44E-BEC5-A85AFD7988DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13740" yWindow="760" windowWidth="16500" windowHeight="17580" xr2:uid="{8EFE0C1B-BAD2-1B45-AB13-3D4AFAD96C4D}"/>
+    <workbookView xWindow="17280" yWindow="920" windowWidth="12800" windowHeight="17280" xr2:uid="{8EFE0C1B-BAD2-1B45-AB13-3D4AFAD96C4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,123 +71,63 @@
     <t>DownloadServerPage_StartTodayModal_TextBox_FirstName</t>
   </si>
   <si>
-    <t>input#FirstName</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_TextBox_FirstName</t>
   </si>
   <si>
-    <t>div#ValidMsgFirstName</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_TextBox_LastName</t>
   </si>
   <si>
-    <t>input#LastName</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_TextBox_LastName</t>
   </si>
   <si>
-    <t>div#ValidMsgLastName</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_TextBox_Email</t>
   </si>
   <si>
-    <t>input#Email</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_TextBox_Email</t>
   </si>
   <si>
-    <t>div#ValidMsgEmail</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_TextBox_PhoneNumber</t>
   </si>
   <si>
-    <t>input#Phone</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_TextBox_PhoneNumber</t>
   </si>
   <si>
-    <t>div#ValidMsgPhone</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_TextBox_CompanyName</t>
   </si>
   <si>
-    <t>input#Company</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_TextBox_Company</t>
   </si>
   <si>
-    <t>div#ValidMsgCompany</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_DropDown_JobTitle</t>
   </si>
   <si>
-    <t>select#jobTitle2</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_Dropdown_JobTitle</t>
   </si>
   <si>
-    <t>div#ValidMsgjobTitle2</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_DropDown_Country</t>
   </si>
   <si>
-    <t>select#Country</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_Dropdown_Country</t>
   </si>
   <si>
-    <t>div#ValidMsgCountry</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_TextBox_Zip</t>
   </si>
   <si>
-    <t>input#PostalCode</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_TextBox_Zip</t>
   </si>
   <si>
-    <t>.mktoError #ValidMsgPostalCode</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_DropDown_Province</t>
   </si>
   <si>
-    <t>select#State</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_Dropdown_Province</t>
   </si>
   <si>
-    <t>.mktoError #ValidMsgState</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_CheckBox_PrivacyPolicy</t>
   </si>
   <si>
-    <t>//input[@id='mktoCheckbox_139299_0']</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_CheckBox_LicenseAgreement</t>
   </si>
   <si>
-    <t>//input[@id='mktoCheckbox_139300_0']</t>
-  </si>
-  <si>
     <t>DownloadServerPage_StartTodayModal_Button_Download</t>
   </si>
   <si>
@@ -252,9 +192,6 @@
   </si>
   <si>
     <t>DownloadServerPage_StartTodayModal_Heading</t>
-  </si>
-  <si>
-    <t>div#modalShow h3</t>
   </si>
   <si>
     <t>div#licenseAgreementDiv h4</t>
@@ -331,9 +268,6 @@
     <t>DownloadServerPage_StartTodayModal_ErrorMessage_Checkbox_TermsAndConditions</t>
   </si>
   <si>
-    <t>div.mktoError #ValidMsgtermsandConditions</t>
-  </si>
-  <si>
     <t>DownloadServerPage_EnterpriseAnalytics_StartTodayModal_CheckBox_LicenseAgreement</t>
   </si>
   <si>
@@ -344,6 +278,72 @@
   </si>
   <si>
     <t>//input[@id='mktoCheckbox_143627_0']</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) select#Country</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) select#jobTitle2</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) select#State</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) div#ValidMsgCountry</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) div#ValidMsgjobTitle2</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) .mktoError #ValidMsgState</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) div#ValidMsgCompany</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) div#ValidMsgEmail</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) div#ValidMsgFirstName</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) div#ValidMsgLastName</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) div#ValidMsgPhone</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) .mktoError #ValidMsgPostalCode</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) input#Company</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) input#Email</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) input#FirstName</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) input#LastName</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) input#Phone</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) input#PostalCode</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) div.mktoError #ValidMsgtermsandConditions</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) .mktoCheckboxList input[name='Double_Opt_in_Compliant__c']</t>
+  </si>
+  <si>
+    <t>form[style]:not([style*="display: none"]) .mktoCheckboxList input[name='termsandConditions']</t>
+  </si>
+  <si>
+    <t>div#modalShow h3</t>
   </si>
 </sst>
 </file>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6CD50A-E106-C04C-9BAE-9E1E25E34BE9}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -775,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -788,10 +788,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -801,10 +801,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -814,10 +814,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -827,10 +827,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -840,10 +840,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -853,10 +853,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -866,10 +866,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -879,10 +879,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -931,10 +931,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -944,10 +944,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -957,10 +957,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -970,10 +970,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -983,10 +983,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -996,10 +996,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1009,10 +1009,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1022,10 +1022,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1035,10 +1035,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1048,10 +1048,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1061,10 +1061,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1074,10 +1074,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1087,10 +1087,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1100,10 +1100,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1113,10 +1113,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1126,10 +1126,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1139,10 +1139,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1152,10 +1152,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1163,10 +1163,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1174,10 +1174,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1185,10 +1185,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1196,10 +1196,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1207,10 +1207,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1218,10 +1218,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1229,10 +1229,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1240,10 +1240,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1251,10 +1251,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1262,10 +1262,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
         <v>10</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1284,10 +1284,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1295,10 +1295,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1306,10 +1306,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1317,10 +1317,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1328,10 +1328,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1339,10 +1339,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,10 +1350,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for Kubernetes and Mobile tab
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/LocatorDictionary/DownloadServerPageLocators.xlsx
+++ b/src/main/resources/CompilerDictionary/LocatorDictionary/DownloadServerPageLocators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/src/main/resources/CompilerDictionary/LocatorDictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02EAAA7-1BDC-C44E-BEC5-A85AFD7988DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12F5198-4BA9-AC45-8B12-419068B497F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="920" windowWidth="12800" windowHeight="17280" xr2:uid="{8EFE0C1B-BAD2-1B45-AB13-3D4AFAD96C4D}"/>
   </bookViews>
@@ -244,9 +244,6 @@
     </r>
   </si>
   <si>
-    <t>ul.downloads-tabs li#mobile&amp;edge</t>
-  </si>
-  <si>
     <t>DownloadPage_Button_AcceptCookies</t>
   </si>
   <si>
@@ -344,6 +341,9 @@
   </si>
   <si>
     <t>div#modalShow h3</t>
+  </si>
+  <si>
+    <t>ul.downloads-tabs li[id='mobile&amp;edge']</t>
   </si>
 </sst>
 </file>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6CD50A-E106-C04C-9BAE-9E1E25E34BE9}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -775,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -788,7 +788,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>63</v>
@@ -801,7 +801,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>64</v>
@@ -814,10 +814,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -827,7 +827,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>62</v>
@@ -1064,7 +1064,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1077,7 +1077,7 @@
         <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1090,7 +1090,7 @@
         <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1103,7 +1103,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1116,7 +1116,7 @@
         <v>20</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1129,7 +1129,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1142,7 +1142,7 @@
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1155,7 +1155,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1166,7 +1166,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1177,7 +1177,7 @@
         <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1188,7 +1188,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1199,7 +1199,7 @@
         <v>11</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1221,7 +1221,7 @@
         <v>17</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1232,7 +1232,7 @@
         <v>25</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1243,7 +1243,7 @@
         <v>51</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1254,7 +1254,7 @@
         <v>18</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>14</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
         <v>10</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1287,7 +1287,7 @@
         <v>12</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1298,7 +1298,7 @@
         <v>16</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1309,7 +1309,7 @@
         <v>24</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1328,10 +1328,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1339,10 +1339,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,10 +1350,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>